<commit_message>
Save current state - employee role integration and UI updates
</commit_message>
<xml_diff>
--- a/writable/temp/Facility_Rental_Report_November_2025.xlsx
+++ b/writable/temp/Facility_Rental_Report_November_2025.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>Reports on Rentals</t>
   </si>
@@ -43,55 +43,43 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Function Hall (ACAD Bldg.)</t>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Prepared by:</t>
+  </si>
+  <si>
+    <t>Noted by:</t>
+  </si>
+  <si>
+    <t>MARY JANE J. CHAVEZ</t>
+  </si>
+  <si>
+    <t>ANGELICA P. REGONDOLA, PhD</t>
+  </si>
+  <si>
+    <t>Rentals-in-Charge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                          AOV -SPMO</t>
+  </si>
+  <si>
+    <t>TOGA ( Lost)</t>
+  </si>
+  <si>
+    <t>Date: JANUARY 2023</t>
+  </si>
+  <si>
+    <t>TOGA (Lost)</t>
+  </si>
+  <si>
+    <t>Please see attached sheet</t>
   </si>
   <si>
     <t>Pls. see attached sheet</t>
-  </si>
-  <si>
-    <t>November 2025</t>
-  </si>
-  <si>
-    <t>University Auditorium</t>
-  </si>
-  <si>
-    <t>University Gymnasium</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Prepared by:</t>
-  </si>
-  <si>
-    <t>Noted by:</t>
-  </si>
-  <si>
-    <t>MARY JANE J. CHAVEZ</t>
-  </si>
-  <si>
-    <t>ANGELICA P. REGONDOLA, PhD</t>
-  </si>
-  <si>
-    <t>Rentals-in-Charge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                          AOV -SPMO</t>
-  </si>
-  <si>
-    <t>TOGA ( Lost)</t>
-  </si>
-  <si>
-    <t>Date: JANUARY 2023</t>
-  </si>
-  <si>
-    <t>TOGA (Lost)</t>
-  </si>
-  <si>
-    <t>Please see attached sheet</t>
   </si>
   <si>
     <t>January 2023</t>
@@ -115,7 +103,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="₱ #,##0.00"/>
+    <numFmt numFmtId="165" formatCode="? #,##0.00"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -217,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -277,11 +265,8 @@
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="17" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
-    <xf xfId="0" fontId="0" numFmtId="165" fillId="2" borderId="1" applyFont="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
     </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
@@ -667,7 +652,7 @@
   <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1" topLeftCell="A4">
-      <selection activeCell="A13" sqref="A13:E13"/>
+      <selection activeCell="A10" sqref="A10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -683,7 +668,7 @@
   <sheetData>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -719,7 +704,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="C8" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="2" customFormat="1">
@@ -740,75 +725,45 @@
       </c>
     </row>
     <row r="10" spans="1:9" customHeight="1" ht="17.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="24">
-        <v>3000.0</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="25">
+        <v>0</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="27"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" customHeight="1" ht="19.5">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="24">
-        <v>15000.0</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" customHeight="1" ht="17.25">
-      <c r="A12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="24">
-        <v>8000.0</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
       <c r="G12" s="14"/>
       <c r="H12" s="15"/>
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" customHeight="1" ht="21.75">
-      <c r="A13" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="26">
-        <v>26000.0</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
       <c r="G13" s="14"/>
       <c r="H13" s="15"/>
       <c r="I13" s="14"/>
@@ -835,7 +790,7 @@
     </row>
     <row r="16" spans="1:9" customHeight="1" ht="14.25">
       <c r="A16" s="11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
@@ -910,7 +865,7 @@
       <c r="C25" s="12"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -960,26 +915,26 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D37" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D41" s="22" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E41" s="22"/>
     </row>
@@ -995,7 +950,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -1004,7 +959,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B85" s="16"/>
       <c r="C85" s="16"/>
@@ -1031,19 +986,19 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="7" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C88" s="8">
         <v>1315</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E88" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:9">
@@ -1125,7 +1080,7 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B100" s="18">
         <f>SUM(C88:C99)</f>
@@ -1137,26 +1092,26 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D106" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>